<commit_message>
force measure display name uniqueness by failing the processing
</commit_message>
<xml_diff>
--- a/spec/files/0_1_09_small_list_incomplete.xlsx
+++ b/spec/files/0_1_09_small_list_incomplete.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="3920" windowWidth="21680" windowHeight="12140" activeTab="3"/>
+    <workbookView xWindow="3920" yWindow="3920" windowWidth="21680" windowHeight="12140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="479">
   <si>
     <t>type</t>
   </si>
@@ -1464,6 +1464,9 @@
   </si>
   <si>
     <t>function group</t>
+  </si>
+  <si>
+    <t>ReduceSpaceInfiltrationByPercentage 2</t>
   </si>
 </sst>
 </file>
@@ -2877,15 +2880,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1233">
@@ -4795,9 +4798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4837,14 +4840,14 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
     </row>
     <row r="2" spans="1:22" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
@@ -5220,7 +5223,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>478</v>
       </c>
       <c r="C14" t="s">
         <v>77</v>
@@ -5973,7 +5976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:G3"/>
     </sheetView>
@@ -6015,50 +6018,50 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
     </row>
     <row r="2" spans="1:22" s="9" customFormat="1" ht="15">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>468</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>469</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>470</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>471</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>472</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>475</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>476</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:22" s="16" customFormat="1" ht="30">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28" t="s">
         <v>473</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>474</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="29" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="28" t="s">
         <v>477</v>
       </c>
       <c r="H3" s="11"/>

</xml_diff>

<commit_message>
write out both formats from excel translator
</commit_message>
<xml_diff>
--- a/spec/files/0_1_09_small_list_incomplete.xlsx
+++ b/spec/files/0_1_09_small_list_incomplete.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="3920" windowWidth="21680" windowHeight="12140" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="480">
   <si>
     <t>type</t>
   </si>
@@ -1467,6 +1467,9 @@
   </si>
   <si>
     <t>ReduceSpaceInfiltrationByPercentage 2</t>
+  </si>
+  <si>
+    <t>Roof Insulation R-value (ft^2*h*R/Btu).</t>
   </si>
 </sst>
 </file>
@@ -1585,8 +1588,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1233">
+  <cellStyleXfs count="1235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2891,7 +2896,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1233">
+  <cellStyles count="1235">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3508,6 +3513,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1228" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1230" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1234" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4124,6 +4130,7 @@
     <cellStyle name="Hyperlink" xfId="1227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4800,7 +4807,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5624,7 +5631,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>267</v>
+        <v>479</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>268</v>

</xml_diff>